<commit_message>
Production Version V1.1 (fixed position list)
</commit_message>
<xml_diff>
--- a/Входящие данные.xlsx
+++ b/Входящие данные.xlsx
@@ -45,7 +45,7 @@
     <t>Регион</t>
   </si>
   <si>
-    <t> 469137733</t>
+    <t>https://www.ozon.ru/brand/karcher-26303230/</t>
   </si>
 </sst>
 </file>
@@ -84,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -120,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -137,6 +143,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -421,7 +428,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,21 +466,19 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="2">
-        <v>334284246</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="2">
-        <v>319020677</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
@@ -483,9 +488,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="2">
-        <v>366308852</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -495,9 +498,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="2">
-        <v>800403479</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -507,9 +508,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="2">
-        <v>810075312</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -519,9 +518,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="2">
-        <v>678425338</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -531,9 +528,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="2">
-        <v>461053252</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -543,9 +538,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="2">
-        <v>375928555</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -555,9 +548,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="2">
-        <v>721358419</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -567,9 +558,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="2">
-        <v>582436053</v>
-      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -579,9 +568,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="2">
-        <v>471785061</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -591,9 +578,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="2">
-        <v>725062412</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -601,11 +586,9 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>

</xml_diff>

<commit_message>
Production Version V1.2 (fixed position list)
</commit_message>
<xml_diff>
--- a/Входящие данные.xlsx
+++ b/Входящие данные.xlsx
@@ -45,7 +45,7 @@
     <t>Регион</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/brand/karcher-26303230/</t>
+    <t>https://www.ozon.ru/seller/ip-yartseva-yu-s-260199/products/?miniapp=seller_260199</t>
   </si>
 </sst>
 </file>
@@ -464,15 +464,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="6"/>
       <c r="H2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Production Version V1.3 (fixed serach requests)
</commit_message>
<xml_diff>
--- a/Входящие данные.xlsx
+++ b/Входящие данные.xlsx
@@ -45,7 +45,7 @@
     <t>Регион</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/seller/ip-yartseva-yu-s-260199/products/?miniapp=seller_260199</t>
+    <t>ежовик гребенчатый</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,16 +464,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>